<commit_message>
update supp tables 4-6 and update Figures 3 and 4 notebook
</commit_message>
<xml_diff>
--- a/dnam-clocks/mFSS-clock/data/processed/tables/Supplementary_table_4_arthritis_coherent_corr_mFSS_model.xlsx
+++ b/dnam-clocks/mFSS-clock/data/processed/tables/Supplementary_table_4_arthritis_coherent_corr_mFSS_model.xlsx
@@ -461,17 +461,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>cg22454769</t>
+          <t>cg00103778</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>26.58930015563965</v>
+        <v>16.45581245422363</v>
       </c>
       <c r="D2" t="n">
-        <v>0.009696744217213591</v>
+        <v>0.001676886618632677</v>
       </c>
       <c r="E2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -480,17 +480,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>cg07553761</t>
+          <t>cg00210249</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>11.71096038818359</v>
+        <v>11.28615665435791</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0007716542648234814</v>
+        <v>0.007270354078367843</v>
       </c>
       <c r="E3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -499,17 +499,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>cg08234504</t>
+          <t>cg00308841</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>13.42937183380127</v>
+        <v>4.345770835876465</v>
       </c>
       <c r="D4" t="n">
-        <v>0.001585134453239076</v>
+        <v>0.001552918698777882</v>
       </c>
       <c r="E4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -518,14 +518,14 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>cg23744638</t>
+          <t>cg00327072</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>10.81192684173584</v>
+        <v>7.449949741363525</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.0004242123099695669</v>
+        <v>0.0001329119683115276</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
@@ -537,14 +537,14 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>cg08128734</t>
+          <t>cg00387658</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>6.267470359802246</v>
+        <v>11.16871929168701</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.00511065555006877</v>
+        <v>0.005229029085042977</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -556,17 +556,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>cg23500537</t>
+          <t>cg00876267</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>39.57051849365234</v>
+        <v>16.26437187194824</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.008744991988104699</v>
+        <v>-0.00246175258406323</v>
       </c>
       <c r="E7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -575,17 +575,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>cg23078123</t>
+          <t>cg01022345</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>17.34835243225098</v>
+        <v>2.746333360671997</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.01534511979713564</v>
+        <v>-0.000836909399607505</v>
       </c>
       <c r="E8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -594,17 +594,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>cg01763090</t>
+          <t>cg01054110</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>46.21932220458984</v>
+        <v>3.781513690948486</v>
       </c>
       <c r="D9" t="n">
-        <v>0.002150119317555146</v>
+        <v>-0.01800887332334671</v>
       </c>
       <c r="E9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -613,17 +613,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>cg01820374</t>
+          <t>cg01447660</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>21.21878242492676</v>
+        <v>2.51879096031189</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.009588283635146142</v>
+        <v>-0.0003632418977135887</v>
       </c>
       <c r="E10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -632,14 +632,14 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>cg09809672</t>
+          <t>cg01763090</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>6.637890338897705</v>
+        <v>46.21932220458984</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.009452983233985492</v>
+        <v>0.002700665955573638</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -651,17 +651,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>cg26161329</t>
+          <t>cg01820374</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>36.30906295776367</v>
+        <v>21.21878242492676</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.004786657149249029</v>
+        <v>-0.0004242123099695669</v>
       </c>
       <c r="E12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -670,17 +670,17 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>cg03431918</t>
+          <t>cg01820962</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>11.10130786895752</v>
+        <v>6.249895095825195</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.004590983072460639</v>
+        <v>-0.02907831121457039</v>
       </c>
       <c r="E13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -689,17 +689,17 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>cg07583137</t>
+          <t>cg01957582</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.9757336974143982</v>
+        <v>9.1905517578125</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.005536332172865991</v>
+        <v>-0.005800029443455991</v>
       </c>
       <c r="E14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -708,14 +708,14 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>cg03607117</t>
+          <t>cg02286081</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>52.72722244262695</v>
+        <v>0.3693400621414185</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.01022224746616661</v>
+        <v>0.002795567134534278</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
@@ -727,14 +727,14 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>cg20273670</t>
+          <t>cg03431918</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>20.48067855834961</v>
+        <v>11.10130786895752</v>
       </c>
       <c r="D16" t="n">
-        <v>0.002700665955573638</v>
+        <v>-0.005536332172865991</v>
       </c>
       <c r="E16" t="b">
         <v>1</v>
@@ -746,17 +746,17 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>cg08415592</t>
+          <t>cg03473532</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>11.88851070404053</v>
+        <v>10.73644351959229</v>
       </c>
       <c r="D17" t="n">
-        <v>0.001676886618632677</v>
+        <v>-0.008744991988104699</v>
       </c>
       <c r="E17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -765,14 +765,14 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>cg09636661</t>
+          <t>cg03485669</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.7440698742866516</v>
+        <v>1.125907182693481</v>
       </c>
       <c r="D18" t="n">
-        <v>0.002795567134534278</v>
+        <v>0.00900697433949915</v>
       </c>
       <c r="E18" t="b">
         <v>0</v>
@@ -784,17 +784,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>cg22026450</t>
+          <t>cg03607117</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>9.459317207336426</v>
+        <v>52.72722244262695</v>
       </c>
       <c r="D19" t="n">
-        <v>0.002841271818186504</v>
+        <v>0.001994860190598691</v>
       </c>
       <c r="E19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -803,17 +803,17 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>cg15894389</t>
+          <t>cg03638795</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>5.895963191986084</v>
+        <v>5.787938594818115</v>
       </c>
       <c r="D20" t="n">
-        <v>0.008921087948501069</v>
+        <v>-0.007713227309632685</v>
       </c>
       <c r="E20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -822,14 +822,14 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>cg03473532</t>
+          <t>cg04064963</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>10.73644351959229</v>
+        <v>5.301578998565674</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.001950712143309977</v>
+        <v>0.004391780451214893</v>
       </c>
       <c r="E21" t="b">
         <v>0</v>
@@ -841,14 +841,14 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>cg06685111</t>
+          <t>cg04200607</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>19.19382286071777</v>
+        <v>12.11180210113525</v>
       </c>
       <c r="D22" t="n">
-        <v>-0.004439712373799597</v>
+        <v>0.0029690109953068</v>
       </c>
       <c r="E22" t="b">
         <v>0</v>
@@ -860,14 +860,14 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>cg01022345</t>
+          <t>cg04208403</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>2.746333360671997</v>
+        <v>14.63229656219482</v>
       </c>
       <c r="D23" t="n">
-        <v>0.003002171894258873</v>
+        <v>-0.01022224746616661</v>
       </c>
       <c r="E23" t="b">
         <v>1</v>
@@ -879,17 +879,17 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>cg19758448</t>
+          <t>cg04416734</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>5.687094211578369</v>
+        <v>22.16415786743164</v>
       </c>
       <c r="D24" t="n">
-        <v>-0.0001414294679278134</v>
+        <v>-0.006669217532218169</v>
       </c>
       <c r="E24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -898,17 +898,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>cg01054110</t>
+          <t>cg04474832</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>3.781513690948486</v>
+        <v>13.95060157775879</v>
       </c>
       <c r="D25" t="n">
-        <v>0.005176359203736492</v>
+        <v>-0.002349385371356845</v>
       </c>
       <c r="E25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -917,14 +917,14 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>cg20816447</t>
+          <t>cg04651240</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>1.036941528320312</v>
+        <v>5.180781364440918</v>
       </c>
       <c r="D26" t="n">
-        <v>0.002967179002980489</v>
+        <v>0.01020169419225591</v>
       </c>
       <c r="E26" t="b">
         <v>0</v>
@@ -936,14 +936,14 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>cg20988565</t>
+          <t>cg04812351</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>10.94745349884033</v>
+        <v>9.005759239196777</v>
       </c>
       <c r="D27" t="n">
-        <v>-0.02124396219396488</v>
+        <v>0.01018109249073571</v>
       </c>
       <c r="E27" t="b">
         <v>0</v>
@@ -955,14 +955,14 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>cg22747507</t>
+          <t>cg04819580</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>1.216158390045166</v>
+        <v>7.345827579498291</v>
       </c>
       <c r="D28" t="n">
-        <v>-0.001136514185383331</v>
+        <v>0.005664501749649536</v>
       </c>
       <c r="E28" t="b">
         <v>0</v>
@@ -974,14 +974,14 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>cg04416734</t>
+          <t>cg05093315</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>22.16415786743164</v>
+        <v>3.272024631500244</v>
       </c>
       <c r="D29" t="n">
-        <v>-0.01244744550538524</v>
+        <v>0.01222342665282773</v>
       </c>
       <c r="E29" t="b">
         <v>0</v>
@@ -993,14 +993,14 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>cg18933331</t>
+          <t>cg05150327</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>33.13585662841797</v>
+        <v>17.9709529876709</v>
       </c>
       <c r="D30" t="n">
-        <v>0.005229029085042977</v>
+        <v>0.001823224494532346</v>
       </c>
       <c r="E30" t="b">
         <v>0</v>
@@ -1012,14 +1012,14 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>cg19761273</t>
+          <t>cg05373251</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>5.924397945404053</v>
+        <v>5.595539093017578</v>
       </c>
       <c r="D31" t="n">
-        <v>-0.001206436239227707</v>
+        <v>0.0120764360460016</v>
       </c>
       <c r="E31" t="b">
         <v>0</v>
@@ -1031,17 +1031,17 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>cg06170683</t>
+          <t>cg05898618</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>2.408959627151489</v>
+        <v>6.514217853546143</v>
       </c>
       <c r="D32" t="n">
-        <v>5.27605898535849e-05</v>
+        <v>-0.002346335233224509</v>
       </c>
       <c r="E32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
@@ -1050,17 +1050,17 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>cg18568843</t>
+          <t>cg06163904</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>13.43373489379883</v>
+        <v>9.85302734375</v>
       </c>
       <c r="D33" t="n">
-        <v>-0.002349385371356845</v>
+        <v>-0.007251287144576408</v>
       </c>
       <c r="E33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -1069,14 +1069,14 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>cg18651026</t>
+          <t>cg06170683</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>20.40043640136719</v>
+        <v>2.408959627151489</v>
       </c>
       <c r="D34" t="n">
-        <v>-0.003357551891713397</v>
+        <v>0.005675958858931156</v>
       </c>
       <c r="E34" t="b">
         <v>0</v>
@@ -1088,17 +1088,17 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>cg04474832</t>
+          <t>cg06400319</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>13.95060157775879</v>
+        <v>4.610074996948242</v>
       </c>
       <c r="D35" t="n">
-        <v>0.01020169419225591</v>
+        <v>-0.0004099065557120618</v>
       </c>
       <c r="E35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -1107,14 +1107,14 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>cg04064963</t>
+          <t>cg06532574</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>5.301578998565674</v>
+        <v>2.327806949615479</v>
       </c>
       <c r="D36" t="n">
-        <v>-0.01980652034468553</v>
+        <v>0.01075252807693089</v>
       </c>
       <c r="E36" t="b">
         <v>0</v>
@@ -1126,17 +1126,17 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>cg18150280</t>
+          <t>cg06540876</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>10.50076770782471</v>
+        <v>1.099820613861084</v>
       </c>
       <c r="D37" t="n">
-        <v>-0.0053441863017426</v>
+        <v>-0.005819265660852338</v>
       </c>
       <c r="E37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -1145,17 +1145,17 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>cg19453093</t>
+          <t>cg06685111</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>2.939518451690674</v>
+        <v>19.19382286071777</v>
       </c>
       <c r="D38" t="n">
-        <v>-0.008448433819395397</v>
+        <v>-0.001109839311006011</v>
       </c>
       <c r="E38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -1164,14 +1164,14 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>cg08761208</t>
+          <t>cg06777902</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>9.644397735595703</v>
+        <v>13.69997119903564</v>
       </c>
       <c r="D39" t="n">
-        <v>0.004448193696663516</v>
+        <v>0.0183799892780891</v>
       </c>
       <c r="E39" t="b">
         <v>0</v>
@@ -1183,14 +1183,14 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>cg17168836</t>
+          <t>cg07553761</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>22.70752906799316</v>
+        <v>11.71096038818359</v>
       </c>
       <c r="D40" t="n">
-        <v>-0.00246175258406323</v>
+        <v>0.001585134453239076</v>
       </c>
       <c r="E40" t="b">
         <v>0</v>
@@ -1202,17 +1202,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>cg18333339</t>
+          <t>cg07583137</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>12.02797317504883</v>
+        <v>0.9757336974143982</v>
       </c>
       <c r="D41" t="n">
-        <v>-0.007713227309632685</v>
+        <v>-0.008448433819395397</v>
       </c>
       <c r="E41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
@@ -1228,7 +1228,7 @@
         <v>1.925208926200867</v>
       </c>
       <c r="D42" t="n">
-        <v>-0.002257297954532452</v>
+        <v>0.005362913181833038</v>
       </c>
       <c r="E42" t="b">
         <v>0</v>
@@ -1240,14 +1240,14 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>cg13039251</t>
+          <t>cg07797372</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>1.658335566520691</v>
+        <v>4.973058223724365</v>
       </c>
       <c r="D43" t="n">
-        <v>-0.001687311217798671</v>
+        <v>0.005176359203736492</v>
       </c>
       <c r="E43" t="b">
         <v>0</v>
@@ -1259,17 +1259,17 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>cg16983588</t>
+          <t>cg08128734</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>1.506835103034973</v>
+        <v>6.267470359802246</v>
       </c>
       <c r="D44" t="n">
-        <v>0.002090306613501207</v>
+        <v>-0.01534511979713564</v>
       </c>
       <c r="E44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -1278,17 +1278,17 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>cg00103778</t>
+          <t>cg08234504</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>16.45581245422363</v>
+        <v>13.42937183380127</v>
       </c>
       <c r="D45" t="n">
-        <v>0.009882934023448342</v>
+        <v>0.002150119317555146</v>
       </c>
       <c r="E45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -1297,17 +1297,17 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>cg16193278</t>
+          <t>cg08236479</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>17.99981117248535</v>
+        <v>5.538629055023193</v>
       </c>
       <c r="D46" t="n">
-        <v>0.007171630998916232</v>
+        <v>-0.002660252357423024</v>
       </c>
       <c r="E46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
@@ -1316,14 +1316,14 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>cg00387658</t>
+          <t>cg08415592</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>11.16871929168701</v>
+        <v>11.88851070404053</v>
       </c>
       <c r="D47" t="n">
-        <v>-0.002303620904771389</v>
+        <v>0.004920865729822138</v>
       </c>
       <c r="E47" t="b">
         <v>0</v>
@@ -1335,17 +1335,17 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>cg20608990</t>
+          <t>cg08713098</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>6.623507976531982</v>
+        <v>14.73132038116455</v>
       </c>
       <c r="D48" t="n">
-        <v>0.0004463825704833901</v>
+        <v>-0.001136514185383331</v>
       </c>
       <c r="E48" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
@@ -1354,17 +1354,17 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>cg20052760</t>
+          <t>cg08761208</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1.335966467857361</v>
+        <v>9.644397735595703</v>
       </c>
       <c r="D49" t="n">
-        <v>0.007276739669399734</v>
+        <v>-0.001257564010430256</v>
       </c>
       <c r="E49" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50">
@@ -1373,14 +1373,14 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>cg14195318</t>
+          <t>cg08877357</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>17.41629600524902</v>
+        <v>1.018538355827332</v>
       </c>
       <c r="D50" t="n">
-        <v>0.0001329119683115276</v>
+        <v>-0.008468687910874868</v>
       </c>
       <c r="E50" t="b">
         <v>1</v>
@@ -1392,14 +1392,14 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>cg07797372</t>
+          <t>cg09164913</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>4.973058223724365</v>
+        <v>9.129258155822754</v>
       </c>
       <c r="D51" t="n">
-        <v>0.004012420123311592</v>
+        <v>0.005700005031944456</v>
       </c>
       <c r="E51" t="b">
         <v>0</v>
@@ -1411,17 +1411,17 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>cg05373251</t>
+          <t>cg09636661</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>5.595539093017578</v>
+        <v>0.7440698742866516</v>
       </c>
       <c r="D52" t="n">
-        <v>-0.006876014822801855</v>
+        <v>-0.02776144404201367</v>
       </c>
       <c r="E52" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53">
@@ -1430,17 +1430,17 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>cg14305711</t>
+          <t>cg09809672</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>9.932062149047852</v>
+        <v>6.637890338897705</v>
       </c>
       <c r="D53" t="n">
-        <v>-0.02466153708334904</v>
+        <v>-0.009452983233985492</v>
       </c>
       <c r="E53" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54">
@@ -1449,17 +1449,17 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>cg01820962</t>
+          <t>cg09884851</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>6.249895095825195</v>
+        <v>1.539428949356079</v>
       </c>
       <c r="D54" t="n">
-        <v>-0.000836909399607505</v>
+        <v>-0.01983715033381946</v>
       </c>
       <c r="E54" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55">
@@ -1468,17 +1468,17 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>cg03638795</t>
+          <t>cg09927651</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>5.787938594818115</v>
+        <v>8.607783317565918</v>
       </c>
       <c r="D55" t="n">
-        <v>-0.001109839311006011</v>
+        <v>-0.007399062087406741</v>
       </c>
       <c r="E55" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56">
@@ -1487,14 +1487,14 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>cg19590421</t>
+          <t>cg10001186</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>1.415639996528625</v>
+        <v>10.53973770141602</v>
       </c>
       <c r="D56" t="n">
-        <v>-0.00310975742213006</v>
+        <v>5.27605898535849e-05</v>
       </c>
       <c r="E56" t="b">
         <v>0</v>
@@ -1506,17 +1506,17 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>cg26210267</t>
+          <t>cg10107473</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>10.8084659576416</v>
+        <v>15.37025165557861</v>
       </c>
       <c r="D57" t="n">
-        <v>0.01017850397104238</v>
+        <v>0.001751543629217293</v>
       </c>
       <c r="E57" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -1525,17 +1525,17 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>cg18406708</t>
+          <t>cg10493324</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>16.5920581817627</v>
+        <v>8.983643531799316</v>
       </c>
       <c r="D58" t="n">
-        <v>-0.005822175996303629</v>
+        <v>-0.007087905954860595</v>
       </c>
       <c r="E58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
@@ -1544,14 +1544,14 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>cg18876270</t>
+          <t>cg11067179</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>3.42124342918396</v>
+        <v>12.0800895690918</v>
       </c>
       <c r="D59" t="n">
-        <v>-0.0032364115153138</v>
+        <v>0.0278215547876167</v>
       </c>
       <c r="E59" t="b">
         <v>0</v>
@@ -1563,14 +1563,14 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>cg10001186</t>
+          <t>cg12667125</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>10.53973770141602</v>
+        <v>22.33480262756348</v>
       </c>
       <c r="D60" t="n">
-        <v>-0.006669217532218169</v>
+        <v>0.0002595938991647706</v>
       </c>
       <c r="E60" t="b">
         <v>0</v>
@@ -1582,17 +1582,17 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>cg04208403</t>
+          <t>cg13021857</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>14.63229656219482</v>
+        <v>1.381436109542847</v>
       </c>
       <c r="D61" t="n">
-        <v>0.005216562473060205</v>
+        <v>-0.008332968202077811</v>
       </c>
       <c r="E61" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62">
@@ -1601,17 +1601,17 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>cg21874213</t>
+          <t>cg13039251</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>26.09503364562988</v>
+        <v>1.658335566520691</v>
       </c>
       <c r="D62" t="n">
-        <v>-0.01473563630268434</v>
+        <v>-0.02466153708334904</v>
       </c>
       <c r="E62" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63">
@@ -1620,17 +1620,17 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>cg06400319</t>
+          <t>cg13278478</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>4.610074996948242</v>
+        <v>0.3897678852081299</v>
       </c>
       <c r="D63" t="n">
-        <v>0.02646795553274799</v>
+        <v>-0.01250036990367249</v>
       </c>
       <c r="E63" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64">
@@ -1639,17 +1639,17 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>cg22213242</t>
+          <t>cg14195318</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>8.632048606872559</v>
+        <v>17.41629600524902</v>
       </c>
       <c r="D64" t="n">
-        <v>0.006907358600831098</v>
+        <v>-0.0001414294679278134</v>
       </c>
       <c r="E64" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65">
@@ -1658,17 +1658,17 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>cg09884851</t>
+          <t>cg14200127</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>1.539428949356079</v>
+        <v>4.341618061065674</v>
       </c>
       <c r="D65" t="n">
-        <v>-0.008468687910874868</v>
+        <v>-0.007298565339911376</v>
       </c>
       <c r="E65" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66">
@@ -1677,17 +1677,17 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>cg05093315</t>
+          <t>cg14209784</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>3.272024631500244</v>
+        <v>13.31827735900879</v>
       </c>
       <c r="D66" t="n">
-        <v>0.01222342665282773</v>
+        <v>-0.002257297954532452</v>
       </c>
       <c r="E66" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67">
@@ -1696,14 +1696,14 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>cg06532574</t>
+          <t>cg14257429</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>2.327806949615479</v>
+        <v>5.671872138977051</v>
       </c>
       <c r="D67" t="n">
-        <v>-0.001737921528021825</v>
+        <v>0.008921087948501069</v>
       </c>
       <c r="E67" t="b">
         <v>0</v>
@@ -1715,17 +1715,17 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>cg10107473</t>
+          <t>cg14296767</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>15.37025165557861</v>
+        <v>0.9571419954299927</v>
       </c>
       <c r="D68" t="n">
-        <v>0.005675958858931156</v>
+        <v>-0.01890285811429028</v>
       </c>
       <c r="E68" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69">
@@ -1734,17 +1734,17 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>cg14747813</t>
+          <t>cg14305711</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>1.009586691856384</v>
+        <v>9.932062149047852</v>
       </c>
       <c r="D69" t="n">
-        <v>-0.007290391046345126</v>
+        <v>-0.004461406320470715</v>
       </c>
       <c r="E69" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70">
@@ -1753,14 +1753,14 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>cg02286081</t>
+          <t>cg14532755</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>0.3693400621414185</v>
+        <v>4.979533195495605</v>
       </c>
       <c r="D70" t="n">
-        <v>-0.008893988362872507</v>
+        <v>0.01584235798101475</v>
       </c>
       <c r="E70" t="b">
         <v>0</v>
@@ -1772,17 +1772,17 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>cg12667125</t>
+          <t>cg14747813</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>22.33480262756348</v>
+        <v>1.009586691856384</v>
       </c>
       <c r="D71" t="n">
-        <v>0.002054286257984248</v>
+        <v>-0.005822175996303629</v>
       </c>
       <c r="E71" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72">
@@ -1791,17 +1791,17 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>cg09164913</t>
+          <t>cg14837598</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>9.129258155822754</v>
+        <v>0.02222535014152527</v>
       </c>
       <c r="D72" t="n">
-        <v>-0.02776144404201367</v>
+        <v>-0.01452914986737312</v>
       </c>
       <c r="E72" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73">
@@ -1810,17 +1810,17 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>cg17621438</t>
+          <t>cg15894389</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>0.780722439289093</v>
+        <v>5.895963191986084</v>
       </c>
       <c r="D73" t="n">
-        <v>-0.0004099065557120618</v>
+        <v>-0.004439712373799597</v>
       </c>
       <c r="E73" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74">
@@ -1829,14 +1829,14 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>cg20303331</t>
+          <t>cg15906794</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>11.80581569671631</v>
+        <v>20.58233261108398</v>
       </c>
       <c r="D74" t="n">
-        <v>0.003874108673155473</v>
+        <v>0.003360578546259976</v>
       </c>
       <c r="E74" t="b">
         <v>0</v>
@@ -1848,14 +1848,14 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>cg05898618</t>
+          <t>cg16047471</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>6.514217853546143</v>
+        <v>18.99142265319824</v>
       </c>
       <c r="D75" t="n">
-        <v>-0.001979167733364652</v>
+        <v>0.005549344392158218</v>
       </c>
       <c r="E75" t="b">
         <v>0</v>
@@ -1867,17 +1867,17 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>cg19936954</t>
+          <t>cg16193278</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>16.35050964355469</v>
+        <v>17.99981117248535</v>
       </c>
       <c r="D76" t="n">
-        <v>0.0003170850199304559</v>
+        <v>-0.001950712143309977</v>
       </c>
       <c r="E76" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77">
@@ -1886,17 +1886,17 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>cg23461714</t>
+          <t>cg16983588</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>11.58076190948486</v>
+        <v>1.506835103034973</v>
       </c>
       <c r="D77" t="n">
-        <v>-0.001257564010430256</v>
+        <v>-0.01664743454519437</v>
       </c>
       <c r="E77" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78">
@@ -1912,7 +1912,7 @@
         <v>13.77622509002686</v>
       </c>
       <c r="D78" t="n">
-        <v>-0.02387056926191676</v>
+        <v>0.007276739669399734</v>
       </c>
       <c r="E78" t="b">
         <v>0</v>
@@ -1924,14 +1924,14 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>cg14257429</t>
+          <t>cg17168836</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>5.671872138977051</v>
+        <v>22.70752906799316</v>
       </c>
       <c r="D79" t="n">
-        <v>0.01974637516442206</v>
+        <v>-0.004786657149249029</v>
       </c>
       <c r="E79" t="b">
         <v>1</v>
@@ -1943,14 +1943,14 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>cg03485669</t>
+          <t>cg17508639</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>1.125907182693481</v>
+        <v>6.613599300384521</v>
       </c>
       <c r="D80" t="n">
-        <v>-0.01800887332334671</v>
+        <v>0.001106724063549518</v>
       </c>
       <c r="E80" t="b">
         <v>0</v>
@@ -1962,17 +1962,17 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>cg04200607</t>
+          <t>cg17621438</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>12.11180210113525</v>
+        <v>0.780722439289093</v>
       </c>
       <c r="D81" t="n">
-        <v>-0.01452914986737312</v>
+        <v>-0.02387056926191676</v>
       </c>
       <c r="E81" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82">
@@ -1981,14 +1981,14 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>cg14209784</t>
+          <t>cg18150280</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>13.31827735900879</v>
+        <v>10.50076770782471</v>
       </c>
       <c r="D82" t="n">
-        <v>0.00900697433949915</v>
+        <v>0.002967179002980489</v>
       </c>
       <c r="E82" t="b">
         <v>0</v>
@@ -2000,14 +2000,14 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>cg26158023</t>
+          <t>cg18333339</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>3.103886842727661</v>
+        <v>12.02797317504883</v>
       </c>
       <c r="D83" t="n">
-        <v>0.004142345545432591</v>
+        <v>0.004012420123311592</v>
       </c>
       <c r="E83" t="b">
         <v>0</v>
@@ -2019,17 +2019,17 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>cg27346545</t>
+          <t>cg18406708</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>1.126347064971924</v>
+        <v>16.5920581817627</v>
       </c>
       <c r="D84" t="n">
-        <v>0.0029690109953068</v>
+        <v>-0.001737921528021825</v>
       </c>
       <c r="E84" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85">
@@ -2038,17 +2038,17 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>cg01447660</t>
+          <t>cg18568843</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>2.51879096031189</v>
+        <v>13.43373489379883</v>
       </c>
       <c r="D85" t="n">
-        <v>0.006375884922918037</v>
+        <v>-0.001979167733364652</v>
       </c>
       <c r="E85" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86">
@@ -2057,14 +2057,14 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>cg00876267</t>
+          <t>cg18651026</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>16.26437187194824</v>
+        <v>20.40043640136719</v>
       </c>
       <c r="D86" t="n">
-        <v>-0.01664743454519437</v>
+        <v>0.003874108673155473</v>
       </c>
       <c r="E86" t="b">
         <v>0</v>
@@ -2076,17 +2076,17 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>cg22112841</t>
+          <t>cg18876270</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>9.560867309570312</v>
+        <v>3.42124342918396</v>
       </c>
       <c r="D87" t="n">
-        <v>-0.01250036990367249</v>
+        <v>-0.001687311217798671</v>
       </c>
       <c r="E87" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88">
@@ -2095,17 +2095,17 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>cg14837598</t>
+          <t>cg18933331</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>0.02222535014152527</v>
+        <v>33.13585662841797</v>
       </c>
       <c r="D88" t="n">
-        <v>-0.0003632418977135887</v>
+        <v>-0.00511065555006877</v>
       </c>
       <c r="E88" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89">
@@ -2114,17 +2114,17 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>cg04651240</t>
+          <t>cg19453093</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>5.180781364440918</v>
+        <v>2.939518451690674</v>
       </c>
       <c r="D89" t="n">
-        <v>-0.01890285811429028</v>
+        <v>-0.01980652034468553</v>
       </c>
       <c r="E89" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90">
@@ -2133,14 +2133,14 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>cg14532755</t>
+          <t>cg19590421</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>4.979533195495605</v>
+        <v>1.415639996528625</v>
       </c>
       <c r="D90" t="n">
-        <v>-0.002660252357423024</v>
+        <v>0.02646795553274799</v>
       </c>
       <c r="E90" t="b">
         <v>0</v>
@@ -2152,14 +2152,14 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>cg19753867</t>
+          <t>cg19593767</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>10.41476917266846</v>
+        <v>0.1831125766038895</v>
       </c>
       <c r="D91" t="n">
-        <v>-0.007087905954860595</v>
+        <v>0.01017850397104238</v>
       </c>
       <c r="E91" t="b">
         <v>0</v>
@@ -2171,17 +2171,17 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>cg13278478</t>
+          <t>cg19753867</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>0.3897678852081299</v>
+        <v>10.41476917266846</v>
       </c>
       <c r="D92" t="n">
-        <v>-0.01213071721038672</v>
+        <v>-0.002303620904771389</v>
       </c>
       <c r="E92" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93">
@@ -2190,14 +2190,14 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>cg06777902</t>
+          <t>cg19758448</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>13.69997119903564</v>
+        <v>5.687094211578369</v>
       </c>
       <c r="D93" t="n">
-        <v>-0.02907831121457039</v>
+        <v>0.0003170850199304559</v>
       </c>
       <c r="E93" t="b">
         <v>0</v>
@@ -2209,17 +2209,17 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>cg16047471</t>
+          <t>cg19761273</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>18.99142265319824</v>
+        <v>5.924397945404053</v>
       </c>
       <c r="D94" t="n">
-        <v>0.005700005031944456</v>
+        <v>-0.009588283635146142</v>
       </c>
       <c r="E94" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95">
@@ -2228,17 +2228,17 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>cg08877357</t>
+          <t>cg19936954</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>1.018538355827332</v>
+        <v>16.35050964355469</v>
       </c>
       <c r="D95" t="n">
-        <v>-0.008332968202077811</v>
+        <v>-0.001206436239227707</v>
       </c>
       <c r="E95" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96">
@@ -2247,14 +2247,14 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>cg05150327</t>
+          <t>cg20052760</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>17.9709529876709</v>
+        <v>1.335966467857361</v>
       </c>
       <c r="D96" t="n">
-        <v>0.001994860190598691</v>
+        <v>-0.007290391046345126</v>
       </c>
       <c r="E96" t="b">
         <v>1</v>
@@ -2266,14 +2266,14 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>cg21962791</t>
+          <t>cg20273670</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>5.989545822143555</v>
+        <v>20.48067855834961</v>
       </c>
       <c r="D97" t="n">
-        <v>-0.01983715033381946</v>
+        <v>0.002841271818186504</v>
       </c>
       <c r="E97" t="b">
         <v>0</v>
@@ -2285,17 +2285,17 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>cg08713098</t>
+          <t>cg20303331</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>14.73132038116455</v>
+        <v>11.80581569671631</v>
       </c>
       <c r="D98" t="n">
-        <v>0.005362913181833038</v>
+        <v>-0.01244744550538524</v>
       </c>
       <c r="E98" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99">
@@ -2304,14 +2304,14 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>cg06540876</t>
+          <t>cg20608990</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>1.099820613861084</v>
+        <v>6.623507976531982</v>
       </c>
       <c r="D99" t="n">
-        <v>0.001751543629217293</v>
+        <v>0.002090306613501207</v>
       </c>
       <c r="E99" t="b">
         <v>0</v>
@@ -2323,14 +2323,14 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>cg21915074</t>
+          <t>cg20816447</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>18.45192337036133</v>
+        <v>1.036941528320312</v>
       </c>
       <c r="D100" t="n">
-        <v>0.001106724063549518</v>
+        <v>0.007171630998916232</v>
       </c>
       <c r="E100" t="b">
         <v>0</v>
@@ -2342,17 +2342,17 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>cg14296767</t>
+          <t>cg20988565</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>0.9571419954299927</v>
+        <v>10.94745349884033</v>
       </c>
       <c r="D101" t="n">
-        <v>0.01075252807693089</v>
+        <v>-0.004590983072460639</v>
       </c>
       <c r="E101" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102">
@@ -2361,14 +2361,14 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>cg01957582</t>
+          <t>cg21585707</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>9.1905517578125</v>
+        <v>1.137237668037415</v>
       </c>
       <c r="D102" t="n">
-        <v>0.005664501749649536</v>
+        <v>0.005657280476731557</v>
       </c>
       <c r="E102" t="b">
         <v>0</v>
@@ -2380,17 +2380,17 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>cg13021857</t>
+          <t>cg21874213</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>1.381436109542847</v>
+        <v>26.09503364562988</v>
       </c>
       <c r="D103" t="n">
-        <v>0.01018109249073571</v>
+        <v>-0.003357551891713397</v>
       </c>
       <c r="E103" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104">
@@ -2399,14 +2399,14 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>cg17508639</t>
+          <t>cg21915074</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>6.613599300384521</v>
+        <v>18.45192337036133</v>
       </c>
       <c r="D104" t="n">
-        <v>0.01584235798101475</v>
+        <v>0.005216562473060205</v>
       </c>
       <c r="E104" t="b">
         <v>0</v>
@@ -2418,14 +2418,14 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>cg06163904</t>
+          <t>cg21962791</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>9.85302734375</v>
+        <v>5.989545822143555</v>
       </c>
       <c r="D105" t="n">
-        <v>-0.005800029443455991</v>
+        <v>0.006375884922918037</v>
       </c>
       <c r="E105" t="b">
         <v>0</v>
@@ -2437,17 +2437,17 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>cg23878906</t>
+          <t>cg22026450</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>1.362079620361328</v>
+        <v>9.459317207336426</v>
       </c>
       <c r="D106" t="n">
-        <v>-0.004461406320470715</v>
+        <v>-0.006876014822801855</v>
       </c>
       <c r="E106" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107">
@@ -2456,14 +2456,14 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>cg22943590</t>
+          <t>cg22040301</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>4.934535980224609</v>
+        <v>0.9168720245361328</v>
       </c>
       <c r="D107" t="n">
-        <v>0.005657280476731557</v>
+        <v>0.002054286257984248</v>
       </c>
       <c r="E107" t="b">
         <v>0</v>
@@ -2475,14 +2475,14 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>cg26424147</t>
+          <t>cg22112841</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>12.46761512756348</v>
+        <v>9.560867309570312</v>
       </c>
       <c r="D108" t="n">
-        <v>0.004920865729822138</v>
+        <v>0.004142345545432591</v>
       </c>
       <c r="E108" t="b">
         <v>0</v>
@@ -2494,14 +2494,14 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>cg00308841</t>
+          <t>cg22213242</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>4.345770835876465</v>
+        <v>8.632048606872559</v>
       </c>
       <c r="D109" t="n">
-        <v>-0.002346335233224509</v>
+        <v>0.01974637516442206</v>
       </c>
       <c r="E109" t="b">
         <v>0</v>
@@ -2513,14 +2513,14 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>cg09927651</t>
+          <t>cg22454769</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>8.607783317565918</v>
+        <v>26.58930015563965</v>
       </c>
       <c r="D110" t="n">
-        <v>0.004391780451214893</v>
+        <v>0.009696744217213591</v>
       </c>
       <c r="E110" t="b">
         <v>0</v>
@@ -2532,14 +2532,14 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>cg00327072</t>
+          <t>cg22747507</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>7.449949741363525</v>
+        <v>1.216158390045166</v>
       </c>
       <c r="D111" t="n">
-        <v>0.001552918698777882</v>
+        <v>0.006907358600831098</v>
       </c>
       <c r="E111" t="b">
         <v>0</v>
@@ -2551,17 +2551,17 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>cg08236479</t>
+          <t>cg22943590</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>5.538629055023193</v>
+        <v>4.934535980224609</v>
       </c>
       <c r="D112" t="n">
-        <v>-0.005819265660852338</v>
+        <v>-0.02124396219396488</v>
       </c>
       <c r="E112" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113">
@@ -2570,17 +2570,17 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>cg27068143</t>
+          <t>cg23078123</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>3.556773900985718</v>
+        <v>17.34835243225098</v>
       </c>
       <c r="D113" t="n">
-        <v>-0.006259382506397853</v>
+        <v>-0.0053441863017426</v>
       </c>
       <c r="E113" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114">
@@ -2589,17 +2589,17 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>cg24667575</t>
+          <t>cg23461714</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>1.963732600212097</v>
+        <v>11.58076190948486</v>
       </c>
       <c r="D114" t="n">
-        <v>0.0120764360460016</v>
+        <v>-0.006259382506397853</v>
       </c>
       <c r="E114" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115">
@@ -2608,14 +2608,14 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>cg22040301</t>
+          <t>cg23500537</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>0.9168720245361328</v>
+        <v>39.57051849365234</v>
       </c>
       <c r="D115" t="n">
-        <v>0.005549344392158218</v>
+        <v>0.0007716542648234814</v>
       </c>
       <c r="E115" t="b">
         <v>0</v>
@@ -2627,17 +2627,17 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>cg04812351</t>
+          <t>cg23744638</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>9.005759239196777</v>
+        <v>10.81192684173584</v>
       </c>
       <c r="D116" t="n">
-        <v>-0.007298565339911376</v>
+        <v>-0.01473563630268434</v>
       </c>
       <c r="E116" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117">
@@ -2646,17 +2646,17 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>cg11067179</t>
+          <t>cg23878906</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>12.0800895690918</v>
+        <v>1.362079620361328</v>
       </c>
       <c r="D117" t="n">
-        <v>0.001823224494532346</v>
+        <v>-0.006225948875288929</v>
       </c>
       <c r="E117" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118">
@@ -2665,14 +2665,14 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>cg14200127</t>
+          <t>cg24667575</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>4.341618061065674</v>
+        <v>1.963732600212097</v>
       </c>
       <c r="D118" t="n">
-        <v>0.0002595938991647706</v>
+        <v>0.009882934023448342</v>
       </c>
       <c r="E118" t="b">
         <v>0</v>
@@ -2684,17 +2684,17 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>cg15906794</t>
+          <t>cg26010412</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>20.58233261108398</v>
+        <v>5.861453533172607</v>
       </c>
       <c r="D119" t="n">
-        <v>-0.007399062087406741</v>
+        <v>-0.008893988362872507</v>
       </c>
       <c r="E119" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120">
@@ -2703,17 +2703,17 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>cg26010412</t>
+          <t>cg26158023</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>5.861453533172607</v>
+        <v>3.103886842727661</v>
       </c>
       <c r="D120" t="n">
-        <v>-0.007251287144576408</v>
+        <v>-0.0032364115153138</v>
       </c>
       <c r="E120" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121">
@@ -2722,17 +2722,17 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>cg19593767</t>
+          <t>cg26161329</t>
         </is>
       </c>
       <c r="C121" t="n">
-        <v>0.1831125766038895</v>
+        <v>36.30906295776367</v>
       </c>
       <c r="D121" t="n">
-        <v>0.0278215547876167</v>
+        <v>0.003002171894258873</v>
       </c>
       <c r="E121" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122">
@@ -2741,14 +2741,14 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>cg21585707</t>
+          <t>cg26210267</t>
         </is>
       </c>
       <c r="C122" t="n">
-        <v>1.137237668037415</v>
+        <v>10.8084659576416</v>
       </c>
       <c r="D122" t="n">
-        <v>0.003360578546259976</v>
+        <v>-0.00310975742213006</v>
       </c>
       <c r="E122" t="b">
         <v>1</v>
@@ -2760,14 +2760,14 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>cg00210249</t>
+          <t>cg26424147</t>
         </is>
       </c>
       <c r="C123" t="n">
-        <v>11.28615665435791</v>
+        <v>12.46761512756348</v>
       </c>
       <c r="D123" t="n">
-        <v>0.0183799892780891</v>
+        <v>0.004448193696663516</v>
       </c>
       <c r="E123" t="b">
         <v>0</v>
@@ -2779,14 +2779,14 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>cg04819580</t>
+          <t>cg27068143</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>7.345827579498291</v>
+        <v>3.556773900985718</v>
       </c>
       <c r="D124" t="n">
-        <v>0.007270354078367843</v>
+        <v>0.0004463825704833901</v>
       </c>
       <c r="E124" t="b">
         <v>0</v>
@@ -2798,17 +2798,17 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>cg10493324</t>
+          <t>cg27346545</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>8.983643531799316</v>
+        <v>1.126347064971924</v>
       </c>
       <c r="D125" t="n">
-        <v>-0.006225948875288929</v>
+        <v>-0.01213071721038672</v>
       </c>
       <c r="E125" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126">

</xml_diff>